<commit_message>
short map gemaakt voor Astrid
</commit_message>
<xml_diff>
--- a/zibs2024/mappable/nl.zorg.MedicationAgreement-v4.0(2024EN).xlsx
+++ b/zibs2024/mappable/nl.zorg.MedicationAgreement-v4.0(2024EN).xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nictiznl-my.sharepoint.com/personal/jacob_engel_nictiz_nl/Documents/Documenten/GitHub/eu-nl-compared/zibs2024/mappable/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_3A11BE8C53B947DF517C261AB2D902F0B0F8EA8C" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{385BD53E-7690-0C4C-91A0-D10F3836D1DB}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="24840" windowHeight="14740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -322,8 +328,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -382,17 +388,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -430,7 +444,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -464,6 +478,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -498,9 +513,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -673,14 +689,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="55.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -709,7 +730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -732,7 +753,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -755,7 +776,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -778,7 +799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -801,7 +822,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -824,7 +845,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -847,7 +868,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -870,7 +891,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -893,7 +914,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -916,7 +937,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -942,7 +963,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -965,7 +986,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -994,7 +1015,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -1023,7 +1044,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1049,7 +1070,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
@@ -1084,6 +1105,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
+    <Inhoud xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BAFAE49EF5FC2A44A9A24B379C77993A" ma:contentTypeVersion="18" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="4e3f09d53704208a567efd423a8e8ffb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b19602bd-a67a-4df8-b412-b401dd608f7a" xmlns:ns3="3af30693-c405-4a5b-908a-bd1dc294f76b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5e8dd9eed0ce6952e5fe39cbc0c50bd" ns2:_="" ns3:_="">
     <xsd:import namespace="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
@@ -1340,35 +1382,46 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="3af30693-c405-4a5b-908a-bd1dc294f76b" xsi:nil="true"/>
-    <Inhoud xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b19602bd-a67a-4df8-b412-b401dd608f7a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812A9B0D-6843-45D9-8B89-3DEF7E704A81}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6423DA3-05AA-4B03-9909-6594711CBF13}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3af30693-c405-4a5b-908a-bd1dc294f76b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{089F9F9D-1D6C-44DF-BDBC-368E5D3DE238}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{089F9F9D-1D6C-44DF-BDBC-368E5D3DE238}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A6423DA3-05AA-4B03-9909-6594711CBF13}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812A9B0D-6843-45D9-8B89-3DEF7E704A81}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b19602bd-a67a-4df8-b412-b401dd608f7a"/>
+    <ds:schemaRef ds:uri="3af30693-c405-4a5b-908a-bd1dc294f76b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>